<commit_message>
added reader for Soco Corpus
</commit_message>
<xml_diff>
--- a/annotador-core/src/main/resources/rules/TEST-ES.xlsx
+++ b/annotador-core/src/main/resources/rules/TEST-ES.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnavas\Desktop\LPS\Annotador\annotador-core\src\main\resources\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnavas\CODE\Annotador\annotador-core\src\main\resources\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$195</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$194</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="183">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -134,12 +134,6 @@
     <t>en mayo me gusta ir con Abril al campo, sobre todo los jueves y los domingos...</t>
   </si>
   <si>
-    <t>Abril es un mes precioso.</t>
-  </si>
-  <si>
-    <t>Abril aqui no debería ser NP</t>
-  </si>
-  <si>
     <t>Abril es una persona maravillosa.</t>
   </si>
   <si>
@@ -570,12 +564,24 @@
   </si>
   <si>
     <t>TEST</t>
+  </si>
+  <si>
+    <t>en &lt;TIMEX3 tid="t1" type="DATE" value="2019-05"&gt;mayo&lt;/TIMEX3&gt; me gusta ir con Abril al campo, sobre todo los &lt;TIMEX3 tid="t2" type="DATE" value="2019-WXX-04"&gt;jueves&lt;/TIMEX3&gt; y los &lt;TIMEX3 tid="t3" type="DATE" value="2019-WXX-07"&gt;domingos&lt;/TIMEX3&gt;...</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>debería anotarlo) afterwards?</t>
+  </si>
+  <si>
+    <t>esa persona hizo lo mismo en el &lt;TIMEX3 tid="t1" type="DATE" value="PAST_REF"&gt;pasado&lt;/TIMEX3&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -626,7 +632,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -888,40 +894,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D180"/>
+  <dimension ref="A1:E179"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D15"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="73.6328125" customWidth="1"/>
+    <col min="3" max="3" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" t="s">
         <v>177</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>178</v>
       </c>
-      <c r="C1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -931,43 +944,58 @@
       <c r="C3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -976,9 +1004,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -987,9 +1015,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -998,31 +1026,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
@@ -1031,9 +1059,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
@@ -1042,9 +1070,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
@@ -1053,9 +1081,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
@@ -1064,9 +1092,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
         <v>0</v>
@@ -1077,7 +1105,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
@@ -1088,7 +1116,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>0</v>
@@ -1099,7 +1127,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
@@ -1110,7 +1138,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
@@ -1121,7 +1149,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
@@ -1132,7 +1160,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>0</v>
@@ -1143,7 +1171,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>0</v>
@@ -1154,7 +1182,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>0</v>
@@ -1165,7 +1193,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
         <v>0</v>
@@ -1176,7 +1204,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
         <v>0</v>
@@ -1187,7 +1215,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
         <v>0</v>
@@ -1198,166 +1226,163 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" t="s">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C39" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="C41" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C42" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C43" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C44" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C45" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>82</v>
+      <c r="A46" s="1">
+        <v>33288</v>
       </c>
       <c r="C46" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
@@ -1365,7 +1390,7 @@
         <v>33288</v>
       </c>
       <c r="C47" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
@@ -1373,7 +1398,7 @@
         <v>33288</v>
       </c>
       <c r="C48" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -1381,7 +1406,7 @@
         <v>33288</v>
       </c>
       <c r="C49" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -1389,31 +1414,31 @@
         <v>33288</v>
       </c>
       <c r="C50" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="1">
-        <v>33288</v>
+      <c r="A51" t="s">
+        <v>62</v>
       </c>
       <c r="C51" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C52" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>65</v>
+      <c r="A53" s="1">
+        <v>33288</v>
       </c>
       <c r="C53" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -1421,7 +1446,7 @@
         <v>33288</v>
       </c>
       <c r="C54" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -1429,7 +1454,7 @@
         <v>33288</v>
       </c>
       <c r="C55" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
@@ -1437,628 +1462,631 @@
         <v>33288</v>
       </c>
       <c r="C56" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" s="1">
-        <v>33288</v>
+      <c r="A57" t="s">
+        <v>64</v>
       </c>
       <c r="C57" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C58" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="C59" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C60" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C61" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C62" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C63" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C64" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C65" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C66" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="C67" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C68" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C69" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C70" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="C71" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C72" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C73" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C74" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C75" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C76" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C77" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C78" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C79" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C80" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C81" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C82" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C83" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C84" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>156</v>
+        <v>53</v>
       </c>
       <c r="C85" t="s">
-        <v>143</v>
+        <v>52</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C86" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C87" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C88" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C89" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C90" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C91" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C92" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C93" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C94" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C95" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C96" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C97" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C98" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C99" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C100" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C101" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C102" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C103" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C104" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C105" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C106" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C107" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C108" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C109" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C110" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C111" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C112" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C113" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C114" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>104</v>
+        <v>156</v>
       </c>
       <c r="C115" t="s">
-        <v>54</v>
+        <v>155</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C116" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C117" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C118" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C119" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C120" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C121" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C122" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C123" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C124" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>167</v>
+        <v>53</v>
       </c>
       <c r="C125" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C126" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C127" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C128" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C129" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C130" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C131" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>61</v>
+        <v>166</v>
       </c>
       <c r="C132" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>168</v>
+        <v>29</v>
+      </c>
+      <c r="B133" t="s">
+        <v>0</v>
       </c>
       <c r="C133" t="s">
-        <v>157</v>
+        <v>28</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B134" t="s">
         <v>0</v>
@@ -2069,10 +2097,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>30</v>
-      </c>
-      <c r="B135" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="C135" t="s">
         <v>28</v>
@@ -2080,7 +2105,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C136" t="s">
         <v>28</v>
@@ -2088,7 +2113,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C137" t="s">
         <v>28</v>
@@ -2096,23 +2121,23 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
+        <v>44</v>
+      </c>
+      <c r="C138" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139" s="1">
+        <v>33288</v>
+      </c>
+      <c r="C139" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
         <v>45</v>
-      </c>
-      <c r="C138" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A139" t="s">
-        <v>46</v>
-      </c>
-      <c r="C139" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A140" s="1">
-        <v>33288</v>
       </c>
       <c r="C140" t="s">
         <v>28</v>
@@ -2120,7 +2145,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C141" t="s">
         <v>28</v>
@@ -2128,7 +2153,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>48</v>
+        <v>133</v>
       </c>
       <c r="C142" t="s">
         <v>28</v>
@@ -2136,7 +2161,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C143" t="s">
         <v>28</v>
@@ -2144,7 +2169,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C144" t="s">
         <v>28</v>
@@ -2152,7 +2177,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C145" t="s">
         <v>28</v>
@@ -2160,7 +2185,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C146" t="s">
         <v>28</v>
@@ -2168,7 +2193,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C147" t="s">
         <v>28</v>
@@ -2176,7 +2201,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C148" t="s">
         <v>28</v>
@@ -2184,7 +2209,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C149" t="s">
         <v>28</v>
@@ -2192,7 +2217,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="C150" t="s">
         <v>28</v>
@@ -2200,7 +2225,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>169</v>
+        <v>127</v>
       </c>
       <c r="C151" t="s">
         <v>28</v>
@@ -2208,7 +2233,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>129</v>
+        <v>168</v>
       </c>
       <c r="C152" t="s">
         <v>28</v>
@@ -2216,7 +2241,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C153" t="s">
         <v>28</v>
@@ -2224,7 +2249,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C154" t="s">
         <v>28</v>
@@ -2232,7 +2257,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C155" t="s">
         <v>28</v>
@@ -2240,7 +2265,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C156" t="s">
         <v>28</v>
@@ -2248,7 +2273,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C157" t="s">
         <v>28</v>
@@ -2256,7 +2281,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C158" t="s">
         <v>28</v>
@@ -2264,168 +2289,160 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>176</v>
+        <v>129</v>
       </c>
       <c r="C159" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C160" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C161" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C162" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="C163" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C164" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C165" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C166" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C167" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C168" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C169" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C170" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C171" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C172" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>124</v>
+        <v>48</v>
       </c>
       <c r="C173" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C174" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C175" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C176" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A177" t="s">
-        <v>53</v>
-      </c>
-      <c r="C177" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A180" t="s">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:C195">
+  <autoFilter ref="A1:C194">
     <sortState ref="A2:C195">
       <sortCondition ref="C1:C195"/>
     </sortState>

</xml_diff>